<commit_message>
Updated For New Mail Seqences
</commit_message>
<xml_diff>
--- a/Data/VisaConfig.xlsx
+++ b/Data/VisaConfig.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rparobot5\Documents\Uipath\VISA_SETTLEMENT_PROCESS\MDB CHARGE BACK\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmpa11194\Documents\UiPath\AA VISA PROCESS\MdbChargeBack Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871FB9C5-9BB5-4303-9A91-BEFE289AA058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C476A79A-0E79-4AD3-84A6-939967000520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{533A41B4-224A-4779-A5C7-3E4B46218A92}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -207,6 +207,15 @@
   </si>
   <si>
     <t>VISA_MDB_DownloadFolderPath</t>
+  </si>
+  <si>
+    <t>Office365ApplicationID</t>
+  </si>
+  <si>
+    <t>Office365ApplicationSecret</t>
+  </si>
+  <si>
+    <t>Office365TenantID</t>
   </si>
 </sst>
 </file>
@@ -754,10 +763,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A79D8F21-4660-448E-8C3A-0D2E91DB482A}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,6 +937,30 @@
         <v>56</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>